<commit_message>
excellib.iferror now works accordingly with graph.py
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -410,15 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1">
         <v>1</v>
       </c>
@@ -445,8 +445,12 @@
         <f>D1:D3&gt;15</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="J1">
+        <f>IFERROR(B1/0, 4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>2</v>
       </c>
@@ -474,7 +478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>3</v>
       </c>
@@ -502,7 +506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:10">
       <c r="B5">
         <v>2</v>
       </c>
@@ -513,7 +517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>4</v>
       </c>
@@ -522,12 +526,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>6</v>
       </c>
@@ -539,12 +543,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:10">
       <c r="B9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:10">
       <c r="B10">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
using named_range in a cell without any operation works correctly
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -15,7 +15,7 @@
     <definedName name="Liste2">Sheet1!$B$1:$B$3</definedName>
     <definedName name="Liste3">Sheet1!$A$17:$G$17</definedName>
   </definedNames>
-  <calcPr calcId="140000" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -416,15 +416,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="L1" sqref="L1:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1">
         <v>1</v>
       </c>
@@ -455,8 +455,12 @@
         <f>IFERROR(B1/0, 4)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="L1">
+        <f>Liste2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>2</v>
       </c>
@@ -487,8 +491,12 @@
         <f>MIN(C1,C2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="L2">
+        <f>Liste2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>3</v>
       </c>
@@ -515,8 +523,12 @@
         <f>D3:D5&gt;15</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L3">
+        <f>Liste2</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="B5">
         <v>2</v>
       </c>
@@ -527,7 +539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>4</v>
       </c>
@@ -536,12 +548,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>6</v>
       </c>
@@ -553,17 +565,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:12">
       <c r="B9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:12">
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>1</v>
       </c>
@@ -594,31 +606,31 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D17">
         <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E17">
         <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
-        <v>80</v>
+        <v>240</v>
       </c>
       <c r="F17">
         <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
-        <v>160</v>
+        <v>480</v>
       </c>
       <c r="G17">
         <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
-        <v>320</v>
+        <v>960</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[bug] fixed offset management
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -8,12 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="indice">Sheet1!$A$16:$G$16</definedName>
     <definedName name="Liste">Sheet1!$A$1:$A$3</definedName>
     <definedName name="Liste2">Sheet1!$B$1:$B$3</definedName>
     <definedName name="Liste3">Sheet1!$A$17:$G$17</definedName>
+    <definedName name="tR">Sheet1!$A1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -416,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L3"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1">
         <v>1</v>
       </c>
@@ -459,8 +461,12 @@
         <f>Liste2</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1">
+        <f>-Liste2</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>2</v>
       </c>
@@ -495,8 +501,12 @@
         <f>Liste2</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2">
+        <f>-Liste2</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>3</v>
       </c>
@@ -527,8 +537,12 @@
         <f>Liste2</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M3">
+        <f>-Liste2</f>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="B5">
         <v>2</v>
       </c>
@@ -539,7 +553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>4</v>
       </c>
@@ -548,12 +562,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>6</v>
       </c>
@@ -565,17 +579,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="B9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>1</v>
       </c>
@@ -631,6 +645,67 @@
       <c r="G17">
         <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
         <v>960</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>13</v>
+      </c>
+      <c r="D24">
+        <v>14</v>
+      </c>
+      <c r="E24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="F26">
+        <f ca="1">SUM(OFFSET(A22:B23,1,0,2,1))</f>
+        <v>17</v>
+      </c>
+      <c r="G26">
+        <f ca="1">OFFSET(A22,1,0)</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -642,4 +717,128 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <f ca="1">OFFSET(Sheet1!A16,0,3)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tests for % case and equality between strings
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -11,11 +11,13 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="indice">Sheet1!$A$16:$G$16</definedName>
+    <definedName name="Indice">Sheet1!$A$16:$G$16</definedName>
+    <definedName name="Input">Sheet1!$A$1</definedName>
     <definedName name="Liste">Sheet1!$A$1:$A$3</definedName>
     <definedName name="Liste2">Sheet1!$B$1:$B$3</definedName>
     <definedName name="Liste3">Sheet1!$A$17:$G$17</definedName>
-    <definedName name="tR">Sheet1!$A1</definedName>
+    <definedName name="Liste4">Sheet1!$C$30:$F$30</definedName>
+    <definedName name="Liste5">Sheet1!$C$31:$F$31</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Romain</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -81,8 +87,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -418,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1">
         <v>1</v>
       </c>
@@ -465,8 +472,12 @@
         <f>-Liste2</f>
         <v>-10</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1">
+        <f>Input</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>2</v>
       </c>
@@ -506,7 +517,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>3</v>
       </c>
@@ -542,7 +553,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="B5">
         <v>2</v>
       </c>
@@ -553,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>4</v>
       </c>
@@ -562,12 +573,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>6</v>
       </c>
@@ -579,17 +590,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="B9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>1</v>
       </c>
@@ -623,27 +634,27 @@
         <v>30</v>
       </c>
       <c r="B17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
         <v>30</v>
       </c>
       <c r="C17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
         <v>60</v>
       </c>
       <c r="D17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
         <v>120</v>
       </c>
       <c r="E17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
         <v>240</v>
       </c>
       <c r="F17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
         <v>480</v>
       </c>
       <c r="G17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
         <v>960</v>
       </c>
     </row>
@@ -706,6 +717,77 @@
       <c r="G26">
         <f ca="1">SUM(OFFSET(A22,0,1):D22)</f>
         <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <f>Liste4*$A$31</f>
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <f>Liste4*$A$31</f>
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <f>Liste4*$A$31</f>
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <f>Liste4*$A$31</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="C32">
+        <f>Liste5 +10</f>
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <f>Liste5 +10</f>
+        <v>14</v>
+      </c>
+      <c r="E32">
+        <f>Liste5 +10</f>
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <f>Liste5 +10</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
+        <f>2%+A36</f>
+        <v>1.02</v>
+      </c>
+      <c r="C37" t="b">
+        <f>C36="David"</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actual string equality check
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -428,7 +428,7 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -785,9 +785,9 @@
         <f>2%+A36</f>
         <v>1.02</v>
       </c>
-      <c r="C37" t="b">
-        <f>C36="David"</f>
-        <v>0</v>
+      <c r="C37">
+        <f>IF(C36="David",1,2)</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
strings are better handled in Range operations and check function "has_operator_or_func_parent" is added to prevent Range outputs when single values needed
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -38,7 +38,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -62,6 +62,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -80,22 +87,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,15 +437,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1">
         <v>1</v>
       </c>
@@ -476,8 +486,12 @@
         <f>Input</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="P1" s="2">
+        <f>IF(Input&gt;1,Liste2,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>2</v>
       </c>
@@ -516,8 +530,12 @@
         <f>-Liste2</f>
         <v>-20</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="P2" s="2">
+        <f>IF(Input&gt;1,Liste2,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>3</v>
       </c>
@@ -552,8 +570,12 @@
         <f>-Liste2</f>
         <v>-30</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="P3" s="2">
+        <f>IF(Input&gt;1,Liste2,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="B5">
         <v>2</v>
       </c>
@@ -564,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>4</v>
       </c>
@@ -573,12 +595,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>6</v>
       </c>
@@ -590,17 +612,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:16">
       <c r="B9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="G9">
+        <f>SUMPRODUCT(Liste2+Liste)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
fixed index parsing on gen_graph
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -439,7 +439,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -655,7 +657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>30</v>
       </c>
@@ -683,8 +685,12 @@
         <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
         <v>960</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="I17">
+        <f>INDEX(Liste,2,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>1</v>
       </c>
@@ -701,7 +707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>6</v>
       </c>
@@ -718,7 +724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>11</v>
       </c>
@@ -735,7 +741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:9">
       <c r="F26">
         <f ca="1">SUM(OFFSET(A22:B23,1,0,2,1))</f>
         <v>17</v>
@@ -745,7 +751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:9">
       <c r="C30">
         <v>1</v>
       </c>
@@ -759,7 +765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>2</v>
       </c>
@@ -780,7 +786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:9">
       <c r="C32">
         <f>Liste5 +10</f>
         <v>12</v>

</xml_diff>

<commit_message>
find_associated_values is able to find when both row and col are the same
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -440,7 +440,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -838,7 +838,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -851,6 +851,10 @@
     <row r="2" spans="1:3">
       <c r="A2">
         <v>2</v>
+      </c>
+      <c r="B2">
+        <f>Liste2</f>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>

<commit_message>
refactoring, eval not good yet
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="EmptyRange">Sheet1!$A$12:$G$12</definedName>
     <definedName name="Indice">Sheet1!$A$16:$G$16</definedName>
     <definedName name="Input">Sheet1!$A$1</definedName>
     <definedName name="Liste">Sheet1!$A$1:$A$3</definedName>
@@ -19,7 +20,7 @@
     <definedName name="Liste4">Sheet1!$C$30:$F$30</definedName>
     <definedName name="Liste5">Sheet1!$C$31:$F$31</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -440,7 +441,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -628,6 +629,36 @@
         <v>9</v>
       </c>
     </row>
+    <row r="13" spans="1:16">
+      <c r="A13">
+        <f>EmptyRange</f>
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <f>EmptyRange</f>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f>EmptyRange</f>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f>EmptyRange</f>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>EmptyRange</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f>EmptyRange</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f>EmptyRange</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="16" spans="1:16">
       <c r="A16">
         <v>1</v>
@@ -834,7 +865,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
first time good eval with IA_PriceExportGas!
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -30,9 +30,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Romain</t>
+  </si>
+  <si>
+    <t>ref</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -453,6 +456,9 @@
       <c r="B1">
         <v>10</v>
       </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
       <c r="D1">
         <f>A1:A3+B1:B3</f>
         <v>11</v>
@@ -623,6 +629,10 @@
         <f>SUMPRODUCT(Liste2+Liste)</f>
         <v>66</v>
       </c>
+      <c r="H9">
+        <f>SUMPRODUCT(Liste*Liste2*(C1:C3=C1))</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:16">
       <c r="B10">
@@ -631,31 +641,31 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13">
-        <f>EmptyRange</f>
+        <f t="shared" ref="A13:G13" si="2">EmptyRange</f>
         <v>0</v>
       </c>
       <c r="B13">
-        <f>EmptyRange</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C13">
-        <f>EmptyRange</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D13">
-        <f>EmptyRange</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E13">
-        <f>EmptyRange</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F13">
-        <f>EmptyRange</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G13">
-        <f>EmptyRange</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -668,23 +678,23 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:G16" si="2">B16+1</f>
+        <f t="shared" ref="C16:G16" si="3">B16+1</f>
         <v>3</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added excellib.vlookup() + tests
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -20,7 +20,7 @@
     <definedName name="Liste4">Sheet1!$C$30:$F$30</definedName>
     <definedName name="Liste5">Sheet1!$C$31:$F$31</definedName>
   </definedNames>
-  <calcPr calcId="140001" calcCompleted="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,12 +30,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Romain</t>
   </si>
   <si>
     <t>ref</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Ringo</t>
+  </si>
+  <si>
+    <t>bass</t>
+  </si>
+  <si>
+    <t>lead guitar</t>
+  </si>
+  <si>
+    <t>rythm guitar</t>
+  </si>
+  <si>
+    <t>drums</t>
   </si>
 </sst>
 </file>
@@ -443,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -706,7 +730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:16">
       <c r="A17">
         <v>30</v>
       </c>
@@ -743,7 +767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:16">
       <c r="A22">
         <v>1</v>
       </c>
@@ -759,8 +783,36 @@
       <c r="E22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="J22" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22">
+        <f>$H$22*20+I22</f>
+        <v>30</v>
+      </c>
+      <c r="N22">
+        <f>VLOOKUP(22,I22:L25,4)</f>
+        <v>40</v>
+      </c>
+      <c r="O22">
+        <f>VLOOKUP(30,I22:L25,4,FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="P22" t="e">
+        <f>VLOOKUP(31,I22:L25,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23">
         <v>6</v>
       </c>
@@ -776,8 +828,21 @@
       <c r="E23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="I23">
+        <v>20</v>
+      </c>
+      <c r="J23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ref="L23:L25" si="4">$H$22*20+I23</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24">
         <v>11</v>
       </c>
@@ -793,8 +858,36 @@
       <c r="E24">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="I24">
+        <v>30</v>
+      </c>
+      <c r="J24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" t="s">
+        <v>7</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="I25">
+        <v>40</v>
+      </c>
+      <c r="J25" t="s">
+        <v>5</v>
+      </c>
+      <c r="K25" t="s">
+        <v>9</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="B26" t="e">
         <f>A22:B24+A22:C22</f>
         <v>#VALUE!</v>
@@ -808,7 +901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:16">
       <c r="C30">
         <v>1</v>
       </c>
@@ -822,7 +915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:16">
       <c r="A31">
         <v>2</v>
       </c>
@@ -843,7 +936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:16">
       <c r="C32">
         <f>Liste5 +10</f>
         <v>12</v>

</xml_diff>

<commit_message>
CHOOSE handled by gen_graph()
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -465,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -976,6 +976,12 @@
       <c r="A39">
         <f t="array" ref="A39">IFERROR(MATCH(TRUE,Liste&gt;2,0),"Rien")</f>
         <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="str">
+        <f>CHOOSE(A1, J22,J23,J24,J25)</f>
+        <v>Paul</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first ideas for graph updates
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -474,7 +474,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="B17" sqref="B17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -741,27 +741,27 @@
         <v>30</v>
       </c>
       <c r="B17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3,1,Indice-1))</f>
         <v>30</v>
       </c>
       <c r="C17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3,1,Indice-1))</f>
         <v>60</v>
       </c>
       <c r="D17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3,1,Indice-1))</f>
         <v>120</v>
       </c>
       <c r="E17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3,1,Indice-1))</f>
         <v>240</v>
       </c>
       <c r="F17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3,1,Indice-1))</f>
         <v>480</v>
       </c>
       <c r="G17">
-        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3, 1, Indice-1))</f>
+        <f>SUM(INDEX(Liste3,1,1):INDEX(Liste3,1,Indice-1))</f>
         <v>960</v>
       </c>
       <c r="I17">

</xml_diff>

<commit_message>
added Spreadsheet.detect_alive() + basic test
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -480,7 +480,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -652,15 +652,6 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>2</v>
-      </c>
-      <c r="P7">
-        <v>3</v>
-      </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8">
@@ -687,18 +678,12 @@
         <v>10</v>
       </c>
       <c r="O9" s="3"/>
-      <c r="P9" s="4">
-        <f>NOP+O10</f>
-        <v>7</v>
-      </c>
+      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16">
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
     </row>
     <row r="11" spans="1:16">
       <c r="P11" s="3"/>
@@ -760,6 +745,10 @@
       <c r="G16">
         <f t="shared" si="3"/>
         <v>7</v>
+      </c>
+      <c r="H16">
+        <f>SUM(INDEX(Indice,1,1):INDEX(Indice,1,A22))</f>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:16">

</xml_diff>

<commit_message>
some cleaning on basic tests
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -480,7 +480,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -676,6 +676,10 @@
       <c r="H9">
         <f>SUMPRODUCT(Liste*Liste2*(C1:C3=C1))</f>
         <v>10</v>
+      </c>
+      <c r="K9" t="str">
+        <f>IF(Input=1,"","Yes")</f>
+        <v/>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="4"/>

</xml_diff>

<commit_message>
Fix the power function (#198)
* Create new function for power

Return excelerror when it fails

* Add tests

* Bugfix

* Add tests

* Rename functions

* Bugfix test
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\workspace\koala\tests\ast\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D50AFFC-774D-4F86-826B-7B6BF0EC3CC6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="680" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +27,14 @@
     <definedName name="Liste5">Sheet1!$C$31:$F$31</definedName>
     <definedName name="NOP">Sheet1!$N$7:$P$7</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -72,9 +84,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -138,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
@@ -152,6 +164,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -476,16 +496,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -536,7 +556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -580,7 +600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -620,7 +640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -631,7 +651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -648,12 +668,12 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -664,8 +684,18 @@
         <f>A6:A8+B8:B10</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <f>J8^K8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
@@ -677,22 +707,26 @@
         <f>SUMPRODUCT(Liste*Liste2*(C1:C3=C1))</f>
         <v>10</v>
       </c>
-      <c r="K9" t="str">
-        <f>IF(Input=1,"","Yes")</f>
-        <v/>
+      <c r="K9" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L9" t="e">
+        <f>J8^K9</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P11" s="3"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ref="A13:G13" si="2">EmptyRange</f>
         <v>0</v>
@@ -722,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -755,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>30</v>
       </c>
@@ -792,7 +826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -837,7 +871,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -867,7 +901,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>11</v>
       </c>
@@ -897,7 +931,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I25">
         <v>40</v>
       </c>
@@ -912,7 +946,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" t="e">
         <f>A22:B24+A22:C22</f>
         <v>#VALUE!</v>
@@ -926,7 +960,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>1</v>
       </c>
@@ -940,7 +974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -964,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C32">
         <f>Liste5 +10</f>
         <v>12</v>
@@ -993,12 +1027,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1006,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f>2%+A36</f>
         <v>1.02</v>
@@ -1016,13 +1050,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="array" ref="A39">IFERROR(MATCH(TRUE,Liste&gt;2,0),"Rien")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>CHOOSE(A1, J22,J23,J24,J25)</f>
         <v>Paul</v>
@@ -1039,21 +1073,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1062,47 +1096,47 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1111,47 +1145,47 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Fix space names sheet (#210)
* Style

* Drop ' from sheetnames

* Add tests
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\workspace\koala\tests\ast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D50AFFC-774D-4F86-826B-7B6BF0EC3CC6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF73054-B405-45B0-8713-A9DF43A948E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet with space" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="EmptyRange">Sheet1!$A$12:$G$12</definedName>
@@ -500,7 +501,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -693,6 +694,10 @@
       <c r="L8">
         <f>J8^K8</f>
         <v>4</v>
+      </c>
+      <c r="N8">
+        <f>'Sheet with space'!A1</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1198,4 +1203,24 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A792A4-5DD3-4E8F-B5D9-EE28883F7256}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>